<commit_message>
up for cham cong
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/DOC_HR1_.xlsx
+++ b/ASP.NET CORE/HRMNS/DOC_HR1_.xlsx
@@ -2,21 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git-Responsitory\DotNet\ASP.NET CORE\HRMNS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\Source\NET CORE\ASP.NET CORE\HRMNS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HR" sheetId="1" r:id="rId1"/>
-    <sheet name="HR sửa" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="CHAM CONG" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="HR sửa" sheetId="3" r:id="rId4"/>
+    <sheet name="HR_MODULE" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="197">
   <si>
     <t>QUẢN LÝ THÔNG TIN NHÂN SỰ</t>
   </si>
@@ -434,13 +436,196 @@
   </si>
   <si>
     <t>TEN BO PHAN</t>
+  </si>
+  <si>
+    <t>Ma BO Phan Chi Tiet</t>
+  </si>
+  <si>
+    <t>Ten Bo Phan Chi Tiet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ma BO Phan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bo phan : CSP -&gt; Ky thuat CSP</t>
+  </si>
+  <si>
+    <t>TECHNICAL</t>
+  </si>
+  <si>
+    <t>- Show danh sách nhân viên</t>
+  </si>
+  <si>
+    <t>- Thêm mới thông tin nhân viên</t>
+  </si>
+  <si>
+    <t>- Chỉnh sửa thông tin nhân viên</t>
+  </si>
+  <si>
+    <t>- Xóa thông tin nhân viên</t>
+  </si>
+  <si>
+    <t>* Khi xóa thông tin nhân viên thì dữ liệu từ các table có con của table nhan vien đều bị xóa đi</t>
+  </si>
+  <si>
+    <t>- update thông tin profile cơ bản</t>
+  </si>
+  <si>
+    <t>- update thông tin sơ yếu lý lịch</t>
+  </si>
+  <si>
+    <t>- update bank info</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>- update liên lạc người thân</t>
+  </si>
+  <si>
+    <t>- update ngày tham gia bảo hiểm xh</t>
+  </si>
+  <si>
+    <t>- Update phép năm</t>
+  </si>
+  <si>
+    <t>- Update thông tin nghi việc</t>
+  </si>
+  <si>
+    <t>-Update kỷ luật LD</t>
+  </si>
+  <si>
+    <t>- Update tình trạng hồ sơ</t>
+  </si>
+  <si>
+    <t>- Update quá trình làm việc</t>
+  </si>
+  <si>
+    <t>- Update thông tin chi trả BH</t>
+  </si>
+  <si>
+    <t>- Update thông tin hợp đồng</t>
+  </si>
+  <si>
+    <t>- Nhắc nhở khi hết hạn hợp đồng</t>
+  </si>
+  <si>
+    <t>-  Import excel thông tin nhân viên, hợp đồng, quá trình làm việc</t>
+  </si>
+  <si>
+    <t>https://www.phanmemchamcong.net/90-san-pham/209-so-do-qui-trinh-cham-cong.html</t>
+  </si>
+  <si>
+    <t>https://fts.com.vn/quan-ly-cham-cong/</t>
+  </si>
+  <si>
+    <t>Phan chia khung gio theo ca</t>
+  </si>
+  <si>
+    <t>- Setting ca lam viec</t>
+  </si>
+  <si>
+    <t>- Setting thoi gian cham di muon, ve som</t>
+  </si>
+  <si>
+    <t>- Luu du lieu cham cong</t>
+  </si>
+  <si>
+    <t>- Setting ngay nghi le</t>
+  </si>
+  <si>
+    <t>- Setting ky tu cham cong.</t>
+  </si>
+  <si>
+    <t>- Dang ky cham cong dac biet</t>
+  </si>
+  <si>
+    <t>- nghi phep</t>
+  </si>
+  <si>
+    <t>- nghi bu</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Dieu chinh cham cong</t>
+  </si>
+  <si>
+    <t>Dieu chinh OT</t>
+  </si>
+  <si>
+    <t>Dieu chinh ngay cong</t>
+  </si>
+  <si>
+    <t>Dieu chinh ho tro</t>
+  </si>
+  <si>
+    <t>- Dang ky nhan vien lam viec theo ca</t>
+  </si>
+  <si>
+    <t>- Dang ky OT</t>
+  </si>
+  <si>
+    <t>- Setting he so tang ca theo gio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select  min(sday) AS IN_TIME,max(sday) AS OUT_TIME, max(nUserID) AS UserId,date_ </t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>SELECT DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') AS SDAY, nUserID,cast(DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') as date) as date_ FROM TB_EVENT_LOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHERE cast (nUserID as varchar) ='2105001' AND </t>
+  </si>
+  <si>
+    <t>--DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') &gt;='2021-03-18' AND DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') &lt;='2021-04-19'</t>
+  </si>
+  <si>
+    <t>cast(DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') as date) in</t>
+  </si>
+  <si>
+    <t>SELECT SDAY FROM(</t>
+  </si>
+  <si>
+    <t>SELECT CAST( DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') AS DATE) AS SDAY, nUserID FROM TB_EVENT_LOG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WHERE cast (nUserID as varchar) ='2105001' --AND </t>
+  </si>
+  <si>
+    <t>--DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') &gt;=@A_CUS_STIME AND DATEADD(s, nDateTime,'1970-01-01 00:00:00.000') &lt;=@A_CUS_FTIME</t>
+  </si>
+  <si>
+    <t>) A</t>
+  </si>
+  <si>
+    <t>GROUP BY SDAY</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>)B</t>
+  </si>
+  <si>
+    <t>group by date_</t>
+  </si>
+  <si>
+    <t>ORDER BY date_ DESC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +679,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -522,7 +715,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -535,10 +728,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -555,6 +752,1199 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>94095</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>180381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="381000"/>
+          <a:ext cx="9238095" cy="4752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>589257</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>84881</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="5524500"/>
+          <a:ext cx="10342857" cy="6752381"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>113295</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>85071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="13525500"/>
+          <a:ext cx="8038095" cy="5228571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>179886</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>94262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10363200" y="13525500"/>
+          <a:ext cx="8714286" cy="7904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>56306</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>190117</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667125" y="171450"/>
+          <a:ext cx="6752381" cy="3066667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>34659</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="381000"/>
+          <a:ext cx="3692258" cy="1000125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3129</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="1905001"/>
+          <a:ext cx="3660729" cy="1600199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129227</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="3810000"/>
+          <a:ext cx="3657600" cy="1653227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>13575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="5905501"/>
+          <a:ext cx="3671174" cy="1200149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>12477</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="7429501"/>
+          <a:ext cx="3670076" cy="2057399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>357371</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="7486650"/>
+          <a:ext cx="4624571" cy="676275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19720</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1209675" y="9906001"/>
+          <a:ext cx="3686845" cy="1733550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>246253</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4991100" y="10048875"/>
+          <a:ext cx="6227953" cy="1581150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>58189</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="12001500"/>
+          <a:ext cx="3715789" cy="1419225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>80180</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486401" y="12001500"/>
+          <a:ext cx="4305299" cy="1413680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>76793</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="13716000"/>
+          <a:ext cx="3705225" cy="1410293"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>20637</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="13716000"/>
+          <a:ext cx="4287837" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>124210</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="15430500"/>
+          <a:ext cx="3686175" cy="1838710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>435611</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486401" y="15430501"/>
+          <a:ext cx="4702810" cy="1752600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>99</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="17716501"/>
+          <a:ext cx="3629025" cy="1323974"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="17716500"/>
+          <a:ext cx="4772025" cy="1381125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>100243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="19431000"/>
+          <a:ext cx="3657600" cy="1433743"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="19431000"/>
+          <a:ext cx="4810125" cy="1514475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>97173</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="21336000"/>
+          <a:ext cx="3629025" cy="1430673"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="21336000"/>
+          <a:ext cx="4905375" cy="1381125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="23241000"/>
+          <a:ext cx="3648075" cy="1381125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="24955501"/>
+          <a:ext cx="3638550" cy="2057400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="24955500"/>
+          <a:ext cx="3124200" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>121404</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219201" y="27470101"/>
+          <a:ext cx="3657599" cy="1797803"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>324927</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5486400" y="27622500"/>
+          <a:ext cx="5201727" cy="1543050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>14175</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1228725" y="29784676"/>
+          <a:ext cx="4257675" cy="1471499"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,8 +2215,8 @@
   </sheetPr>
   <dimension ref="B2:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:L26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,12 +2255,12 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>94</v>
       </c>
     </row>
@@ -1077,7 +2467,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="5" t="s">
         <v>111</v>
       </c>
@@ -1089,7 +2479,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="5" t="s">
         <v>112</v>
       </c>
@@ -1441,9 +2831,11 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
+    <hyperlink ref="C10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1452,10 +2844,209 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
+  <dimension ref="A1:A70"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="P95" sqref="P95"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="B3:Q40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="P23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="P24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="P25" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E26" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E27" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>173</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q37" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q38" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q39" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q40" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="B2:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,13 +3085,13 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -1561,7 +3152,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C17" s="8" t="s">
         <v>11</v>
       </c>
@@ -1572,12 +3163,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1598,7 +3189,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>13</v>
       </c>
@@ -1619,7 +3210,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>14</v>
       </c>
@@ -1640,7 +3231,7 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C23" s="7" t="s">
         <v>110</v>
       </c>
@@ -1658,7 +3249,7 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>15</v>
       </c>
@@ -1675,7 +3266,7 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>26</v>
       </c>
@@ -1689,12 +3280,17 @@
       <c r="K25" s="7"/>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="7"/>
+      <c r="N25" s="7" t="s">
+        <v>140</v>
+      </c>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="R25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
         <v>27</v>
       </c>
@@ -1709,11 +3305,13 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
-      <c r="O26" s="7"/>
+      <c r="O26" s="7" t="s">
+        <v>136</v>
+      </c>
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
         <v>28</v>
       </c>
@@ -1728,11 +3326,13 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
-      <c r="O27" s="7"/>
+      <c r="O27" s="7" t="s">
+        <v>137</v>
+      </c>
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
@@ -1745,11 +3345,13 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
+      <c r="O28" s="7" t="s">
+        <v>138</v>
+      </c>
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
         <v>30</v>
       </c>
@@ -1766,12 +3368,12 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C31" s="5" t="s">
         <v>31</v>
       </c>
@@ -1779,7 +3381,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C32" s="5" t="s">
         <v>32</v>
       </c>
@@ -1791,7 +3393,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
+      <c r="B33" s="17"/>
       <c r="C33" s="7" t="s">
         <v>111</v>
       </c>
@@ -1803,7 +3405,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
+      <c r="B34" s="17"/>
       <c r="C34" s="7" t="s">
         <v>112</v>
       </c>
@@ -1870,7 +3472,7 @@
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="9"/>
@@ -1879,7 +3481,7 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D41" s="9"/>
@@ -1909,7 +3511,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="12" t="s">
         <v>52</v>
       </c>
       <c r="D44" s="9"/>
@@ -1921,7 +3523,7 @@
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="12" t="s">
         <v>53</v>
       </c>
       <c r="D45" s="9"/>
@@ -1936,7 +3538,7 @@
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>114</v>
       </c>
       <c r="D46" s="9"/>
@@ -1951,7 +3553,7 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="12" t="s">
         <v>115</v>
       </c>
       <c r="D47" s="9"/>
@@ -1966,7 +3568,7 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="12" t="s">
         <v>116</v>
       </c>
       <c r="D48" s="9"/>
@@ -1981,7 +3583,7 @@
       </c>
     </row>
     <row r="49" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="12" t="s">
         <v>117</v>
       </c>
       <c r="D49" s="9"/>
@@ -1996,7 +3598,7 @@
       </c>
     </row>
     <row r="50" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="12" t="s">
         <v>118</v>
       </c>
       <c r="D50" s="9"/>
@@ -2188,20 +3790,124 @@
     <hyperlink ref="C6" r:id="rId3"/>
     <hyperlink ref="C7" r:id="rId4"/>
     <hyperlink ref="C8" r:id="rId5"/>
+    <hyperlink ref="C9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:L167"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="F169" sqref="F169"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B72" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L73" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="13" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="13" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="13" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>